<commit_message>
add marcket cap to price
</commit_message>
<xml_diff>
--- a/database/industries/ghaza/ghesalem/balancesheet/quarterly.xlsx
+++ b/database/industries/ghaza/ghesalem/balancesheet/quarterly.xlsx
@@ -188,8 +188,8 @@
     <col min="2" max="2" width="67" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="29" customWidth="1"/>
-    <col min="5" max="5" width="29" customWidth="1"/>
-    <col min="6" max="6" width="31" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="29" customWidth="1"/>
     <col min="7" max="7" width="29" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
   </cols>
@@ -245,7 +245,7 @@
     <row r="3">
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>Copyright @2015 - 2022</t>
+          <t>Copyright @2015 - 2023</t>
         </is>
       </c>
       <c r="C3" s="2">
@@ -374,27 +374,27 @@
       </c>
       <c r="D8" s="7" t="inlineStr">
         <is>
-          <t>فصل دوم منتهی به 1400/06</t>
+          <t>فصل سوم منتهی به 1400/09</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>فصل سوم منتهی به 1400/09</t>
+          <t>فصل چهارم منتهی به 1400/12</t>
         </is>
       </c>
       <c r="F8" s="7" t="inlineStr">
         <is>
-          <t>فصل چهارم منتهی به 1400/12</t>
+          <t>فصل اول منتهی به 1401/03</t>
         </is>
       </c>
       <c r="G8" s="7" t="inlineStr">
         <is>
-          <t>فصل اول منتهی به 1401/03</t>
+          <t>فصل دوم منتهی به 1401/06</t>
         </is>
       </c>
       <c r="H8" s="7" t="inlineStr">
         <is>
-          <t>فصل دوم منتهی به 1401/06</t>
+          <t>فصل سوم منتهی به 1401/09</t>
         </is>
       </c>
     </row>
@@ -409,27 +409,27 @@
       </c>
       <c r="D9" s="10" t="inlineStr">
         <is>
-          <t>1400-08-25 (2)</t>
+          <t>1400-10-29</t>
         </is>
       </c>
       <c r="E9" s="10" t="inlineStr">
         <is>
-          <t>1400-10-29</t>
+          <t>1401-10-29 (6)</t>
         </is>
       </c>
       <c r="F9" s="10" t="inlineStr">
         <is>
-          <t>1401-08-25 (5)</t>
+          <t>1401-04-28</t>
         </is>
       </c>
       <c r="G9" s="10" t="inlineStr">
         <is>
-          <t>1401-04-28</t>
+          <t>1401-08-25 (2)</t>
         </is>
       </c>
       <c r="H9" s="10" t="inlineStr">
         <is>
-          <t>1401-08-25 (2)</t>
+          <t>1401-10-29</t>
         </is>
       </c>
     </row>
@@ -491,19 +491,19 @@
         <v/>
       </c>
       <c r="D12" s="16">
-        <v>27220</v>
+        <v>199788</v>
       </c>
       <c r="E12" s="16">
-        <v>199788</v>
+        <v>124711</v>
       </c>
       <c r="F12" s="16">
-        <v>124711</v>
+        <v>69166</v>
       </c>
       <c r="G12" s="16">
-        <v>69166</v>
+        <v>548992</v>
       </c>
       <c r="H12" s="16">
-        <v>548992</v>
+        <v>41389</v>
       </c>
     </row>
     <row r="13">
@@ -541,19 +541,19 @@
         <v/>
       </c>
       <c r="D14" s="16">
-        <v>1322766</v>
+        <v>1417184</v>
       </c>
       <c r="E14" s="16">
-        <v>1417184</v>
+        <v>1298799</v>
       </c>
       <c r="F14" s="16">
-        <v>1298799</v>
+        <v>2115298</v>
       </c>
       <c r="G14" s="16">
-        <v>2115298</v>
+        <v>3035354</v>
       </c>
       <c r="H14" s="16">
-        <v>3035354</v>
+        <v>4658376</v>
       </c>
     </row>
     <row r="15">
@@ -566,19 +566,19 @@
         <v/>
       </c>
       <c r="D15" s="12">
-        <v>644099</v>
+        <v>685158</v>
       </c>
       <c r="E15" s="12">
-        <v>685158</v>
+        <v>680684</v>
       </c>
       <c r="F15" s="12">
-        <v>680684</v>
+        <v>1389433</v>
       </c>
       <c r="G15" s="12">
-        <v>1389433</v>
+        <v>1206243</v>
       </c>
       <c r="H15" s="12">
-        <v>1206243</v>
+        <v>1373110</v>
       </c>
     </row>
     <row r="16">
@@ -591,19 +591,19 @@
         <v/>
       </c>
       <c r="D16" s="16">
-        <v>147025</v>
+        <v>204791</v>
       </c>
       <c r="E16" s="16">
-        <v>204791</v>
+        <v>693571</v>
       </c>
       <c r="F16" s="16">
-        <v>693571</v>
+        <v>209930</v>
       </c>
       <c r="G16" s="16">
-        <v>209930</v>
+        <v>105015</v>
       </c>
       <c r="H16" s="16">
-        <v>105015</v>
+        <v>312655</v>
       </c>
     </row>
     <row r="17">
@@ -641,19 +641,19 @@
         <v/>
       </c>
       <c r="D18" s="18">
-        <v>2141110</v>
+        <v>2506921</v>
       </c>
       <c r="E18" s="18">
-        <v>2506921</v>
+        <v>2797765</v>
       </c>
       <c r="F18" s="18">
-        <v>2797765</v>
+        <v>3783827</v>
       </c>
       <c r="G18" s="18">
-        <v>3783827</v>
+        <v>4895604</v>
       </c>
       <c r="H18" s="18">
-        <v>4895604</v>
+        <v>6385530</v>
       </c>
     </row>
     <row r="19">
@@ -741,19 +741,19 @@
         <v/>
       </c>
       <c r="D22" s="16">
-        <v>4420163</v>
+        <v>4382650</v>
       </c>
       <c r="E22" s="16">
-        <v>4382650</v>
+        <v>4485773</v>
       </c>
       <c r="F22" s="16">
-        <v>4485773</v>
+        <v>4448774</v>
       </c>
       <c r="G22" s="16">
-        <v>4448774</v>
+        <v>4441313</v>
       </c>
       <c r="H22" s="16">
-        <v>4441313</v>
+        <v>4431833</v>
       </c>
     </row>
     <row r="23">
@@ -851,19 +851,19 @@
         <v/>
       </c>
       <c r="D26" s="18">
-        <v>4421534</v>
+        <v>4384021</v>
       </c>
       <c r="E26" s="18">
-        <v>4384021</v>
+        <v>4487144</v>
       </c>
       <c r="F26" s="18">
-        <v>4487144</v>
+        <v>4450145</v>
       </c>
       <c r="G26" s="18">
-        <v>4450145</v>
+        <v>4442684</v>
       </c>
       <c r="H26" s="18">
-        <v>4442684</v>
+        <v>4433204</v>
       </c>
     </row>
     <row r="27">
@@ -876,19 +876,19 @@
         <v/>
       </c>
       <c r="D27" s="20">
-        <v>6562644</v>
+        <v>6890942</v>
       </c>
       <c r="E27" s="20">
-        <v>6890942</v>
+        <v>7284909</v>
       </c>
       <c r="F27" s="20">
-        <v>7284909</v>
+        <v>8233972</v>
       </c>
       <c r="G27" s="20">
-        <v>8233972</v>
+        <v>9338288</v>
       </c>
       <c r="H27" s="20">
-        <v>9338288</v>
+        <v>10818734</v>
       </c>
     </row>
     <row r="28">
@@ -926,19 +926,19 @@
         <v/>
       </c>
       <c r="D29" s="16">
-        <v>422459</v>
+        <v>529206</v>
       </c>
       <c r="E29" s="16">
-        <v>529206</v>
+        <v>327294</v>
       </c>
       <c r="F29" s="16">
-        <v>327294</v>
+        <v>773044</v>
       </c>
       <c r="G29" s="16">
-        <v>773044</v>
+        <v>812952</v>
       </c>
       <c r="H29" s="16">
-        <v>812952</v>
+        <v>878852</v>
       </c>
     </row>
     <row r="30">
@@ -1011,19 +1011,19 @@
         <v/>
       </c>
       <c r="D32" s="12">
-        <v>147534</v>
+        <v>172675</v>
       </c>
       <c r="E32" s="12">
-        <v>172675</v>
+        <v>147625</v>
       </c>
       <c r="F32" s="12">
-        <v>147625</v>
+        <v>227816</v>
       </c>
       <c r="G32" s="12">
-        <v>227816</v>
+        <v>364392</v>
       </c>
       <c r="H32" s="12">
-        <v>364392</v>
+        <v>472171</v>
       </c>
     </row>
     <row r="33">
@@ -1036,19 +1036,19 @@
         <v/>
       </c>
       <c r="D33" s="16">
-        <v>229475</v>
+        <v>133482</v>
       </c>
       <c r="E33" s="16">
-        <v>133482</v>
+        <v>8819</v>
       </c>
       <c r="F33" s="16">
-        <v>8819</v>
+        <v>8724</v>
       </c>
       <c r="G33" s="16">
-        <v>8724</v>
+        <v>455208</v>
       </c>
       <c r="H33" s="16">
-        <v>455208</v>
+        <v>263834</v>
       </c>
     </row>
     <row r="34">
@@ -1061,19 +1061,19 @@
         <v/>
       </c>
       <c r="D34" s="12">
-        <v>45386</v>
+        <v>38575</v>
       </c>
       <c r="E34" s="12">
-        <v>38575</v>
+        <v>532549</v>
       </c>
       <c r="F34" s="12">
-        <v>532549</v>
+        <v>402903</v>
       </c>
       <c r="G34" s="12">
-        <v>402903</v>
+        <v>416876</v>
       </c>
       <c r="H34" s="12">
-        <v>416876</v>
+        <v>1078754</v>
       </c>
     </row>
     <row r="35">
@@ -1136,19 +1136,19 @@
         <v/>
       </c>
       <c r="D37" s="18">
-        <v>844854</v>
+        <v>873938</v>
       </c>
       <c r="E37" s="18">
-        <v>873938</v>
+        <v>1016287</v>
       </c>
       <c r="F37" s="18">
-        <v>1016287</v>
+        <v>1412487</v>
       </c>
       <c r="G37" s="18">
-        <v>1412487</v>
+        <v>2049428</v>
       </c>
       <c r="H37" s="18">
-        <v>2049428</v>
+        <v>2693611</v>
       </c>
     </row>
     <row r="38">
@@ -1221,7 +1221,7 @@
         <v/>
       </c>
       <c r="D40" s="12">
-        <v>4032</v>
+        <v>0</v>
       </c>
       <c r="E40" s="12">
         <v>0</v>
@@ -1246,19 +1246,19 @@
         <v/>
       </c>
       <c r="D41" s="16">
-        <v>170541</v>
+        <v>221949</v>
       </c>
       <c r="E41" s="16">
-        <v>221949</v>
+        <v>250921</v>
       </c>
       <c r="F41" s="16">
-        <v>250921</v>
+        <v>291630</v>
       </c>
       <c r="G41" s="16">
-        <v>291630</v>
+        <v>332557</v>
       </c>
       <c r="H41" s="16">
-        <v>332557</v>
+        <v>365179</v>
       </c>
     </row>
     <row r="42">
@@ -1271,19 +1271,19 @@
         <v/>
       </c>
       <c r="D42" s="20">
-        <v>174573</v>
+        <v>221949</v>
       </c>
       <c r="E42" s="20">
-        <v>221949</v>
+        <v>250921</v>
       </c>
       <c r="F42" s="20">
-        <v>250921</v>
+        <v>291630</v>
       </c>
       <c r="G42" s="20">
-        <v>291630</v>
+        <v>332557</v>
       </c>
       <c r="H42" s="20">
-        <v>332557</v>
+        <v>365179</v>
       </c>
     </row>
     <row r="43">
@@ -1296,19 +1296,19 @@
         <v/>
       </c>
       <c r="D43" s="18">
-        <v>1019427</v>
+        <v>1095887</v>
       </c>
       <c r="E43" s="18">
-        <v>1095887</v>
+        <v>1267208</v>
       </c>
       <c r="F43" s="18">
-        <v>1267208</v>
+        <v>1704117</v>
       </c>
       <c r="G43" s="18">
-        <v>1704117</v>
+        <v>2381985</v>
       </c>
       <c r="H43" s="18">
-        <v>2381985</v>
+        <v>3058790</v>
       </c>
     </row>
     <row r="44">
@@ -1471,19 +1471,19 @@
         <v/>
       </c>
       <c r="D50" s="12">
-        <v>73529</v>
+        <v>86121</v>
       </c>
       <c r="E50" s="12">
-        <v>86121</v>
+        <v>97253</v>
       </c>
       <c r="F50" s="12">
-        <v>97253</v>
+        <v>122861</v>
       </c>
       <c r="G50" s="12">
-        <v>122861</v>
+        <v>166603</v>
       </c>
       <c r="H50" s="12">
-        <v>166603</v>
+        <v>206785</v>
       </c>
     </row>
     <row r="51">
@@ -1556,19 +1556,19 @@
         <v/>
       </c>
       <c r="D53" s="16">
-        <v>18025</v>
+        <v>17862</v>
       </c>
       <c r="E53" s="16">
-        <v>17862</v>
+        <v>17827</v>
       </c>
       <c r="F53" s="16">
-        <v>17827</v>
+        <v>17696</v>
       </c>
       <c r="G53" s="16">
-        <v>17696</v>
+        <v>17502</v>
       </c>
       <c r="H53" s="16">
-        <v>17502</v>
+        <v>17042</v>
       </c>
     </row>
     <row r="54">
@@ -1641,19 +1641,19 @@
         <v/>
       </c>
       <c r="D56" s="12">
-        <v>954768</v>
+        <v>1194177</v>
       </c>
       <c r="E56" s="12">
-        <v>1194177</v>
+        <v>1405726</v>
       </c>
       <c r="F56" s="12">
-        <v>1405726</v>
+        <v>1892403</v>
       </c>
       <c r="G56" s="12">
-        <v>1892403</v>
+        <v>2275303</v>
       </c>
       <c r="H56" s="12">
-        <v>2275303</v>
+        <v>3039222</v>
       </c>
     </row>
     <row r="57">
@@ -1666,19 +1666,19 @@
         <v/>
       </c>
       <c r="D57" s="18">
-        <v>5543217</v>
+        <v>5795055</v>
       </c>
       <c r="E57" s="18">
-        <v>5795055</v>
+        <v>6017701</v>
       </c>
       <c r="F57" s="18">
-        <v>6017701</v>
+        <v>6529855</v>
       </c>
       <c r="G57" s="18">
-        <v>6529855</v>
+        <v>6956303</v>
       </c>
       <c r="H57" s="18">
-        <v>6956303</v>
+        <v>7759944</v>
       </c>
     </row>
     <row r="58">
@@ -1691,19 +1691,19 @@
         <v/>
       </c>
       <c r="D58" s="20">
-        <v>6562644</v>
+        <v>6890942</v>
       </c>
       <c r="E58" s="20">
-        <v>6890942</v>
+        <v>7284909</v>
       </c>
       <c r="F58" s="20">
-        <v>7284909</v>
+        <v>8233972</v>
       </c>
       <c r="G58" s="20">
-        <v>8233972</v>
+        <v>9338288</v>
       </c>
       <c r="H58" s="20">
-        <v>9338288</v>
+        <v>10818734</v>
       </c>
     </row>
     <row r="59">

</xml_diff>